<commit_message>
Add logic to find images that cause error
</commit_message>
<xml_diff>
--- a/Lab1/RF_data.xlsx
+++ b/Lab1/RF_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\carta\Desktop\Labs_SYS800\SYS800_labs\Lab1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2CD5C8E-0A04-4788-A597-B8D7566617F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14338B8A-FCE9-4634-ADF0-AB339A76DEB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{56D74342-AB77-4321-A8CB-730300F98D54}"/>
+    <workbookView minimized="1" xWindow="33000" yWindow="2235" windowWidth="21600" windowHeight="9975" firstSheet="2" activeTab="2" xr2:uid="{56D74342-AB77-4321-A8CB-730300F98D54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="19">
   <si>
     <t>num trees</t>
   </si>
@@ -140,7 +140,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -148,12 +148,325 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -162,16 +475,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4863,7 +5221,34 @@
     </cx:data>
   </cx:chartData>
   <cx:chart>
-    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Distribution des erreurs</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>Distribution des erreurs</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
     <cx:plotArea>
       <cx:plotAreaRegion>
         <cx:series layoutId="clusteredColumn" uniqueId="{03E6A86A-F62D-4B06-B5AC-C68D96DD8818}">
@@ -4875,10 +5260,66 @@
       </cx:plotAreaRegion>
       <cx:axis id="0">
         <cx:catScaling gapWidth="0"/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Classe</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                </a:rPr>
+                <a:t>Classe</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
         <cx:valScaling/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Nombre d'erreurs de classification</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                </a:rPr>
+                <a:t>Nombre d'erreurs de classification</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
         <cx:majorGridlines/>
         <cx:tickLabels/>
       </cx:axis>
@@ -4900,7 +5341,34 @@
     </cx:data>
   </cx:chartData>
   <cx:chart>
-    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Distribution des erreurs pour LBP</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>Distribution des erreurs pour LBP</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
     <cx:plotArea>
       <cx:plotAreaRegion>
         <cx:series layoutId="clusteredColumn" uniqueId="{03E6A86A-F62D-4B06-B5AC-C68D96DD8818}">
@@ -4912,10 +5380,66 @@
       </cx:plotAreaRegion>
       <cx:axis id="0">
         <cx:catScaling gapWidth="0"/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Classe</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                </a:rPr>
+                <a:t>Classe</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
         <cx:valScaling/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Nombre d'erreurs de classification</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                </a:rPr>
+                <a:t>Nombre d'erreurs de classification</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
         <cx:majorGridlines/>
         <cx:tickLabels/>
       </cx:axis>
@@ -8237,15 +8761,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>536864</xdr:colOff>
+      <xdr:colOff>392207</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>39</xdr:col>
-      <xdr:colOff>470647</xdr:colOff>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>324971</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>142876</xdr:rowOff>
+      <xdr:rowOff>156882</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8403,8 +8927,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="1828800" y="2986086"/>
-              <a:ext cx="7324725" cy="4691063"/>
+              <a:off x="647700" y="3005136"/>
+              <a:ext cx="3981450" cy="4691063"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -8486,8 +9010,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="1819275" y="2647950"/>
-              <a:ext cx="7324725" cy="4691063"/>
+              <a:off x="647700" y="2667000"/>
+              <a:ext cx="3790950" cy="4691063"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -8819,8 +9343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D85EC1C0-8344-47F3-85E9-126F18894993}">
   <dimension ref="A1:R205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AO37" sqref="AO37"/>
+    <sheetView topLeftCell="J10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y15" sqref="Y15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8839,20 +9363,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="G1" s="6" t="s">
+      <c r="A1" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="G1" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -8885,14 +9409,14 @@
       <c r="K2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="O2" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6" t="s">
+      <c r="P2" s="27"/>
+      <c r="Q2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="R2" s="6"/>
+      <c r="R2" s="27"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -13029,7 +13553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3762B2B5-446D-47A9-92F5-E559D604660E}">
   <dimension ref="A1:K205"/>
   <sheetViews>
-    <sheetView topLeftCell="E10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="E13" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -13047,20 +13571,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="G1" s="6" t="s">
+      <c r="A1" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="G1" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -17164,510 +17688,527 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D1DAF9C-CD9B-4EAA-B358-F970624806A6}">
   <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="12" width="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C1" s="8" t="s">
+      <c r="A1" s="11"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C2" s="4">
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="36" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="15">
         <v>0</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="8">
         <v>1</v>
       </c>
-      <c r="E2" s="4">
-        <v>2</v>
-      </c>
-      <c r="F2" s="4">
+      <c r="E2" s="8">
+        <v>2</v>
+      </c>
+      <c r="F2" s="8">
         <v>3</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="8">
         <v>4</v>
       </c>
-      <c r="H2" s="4">
-        <v>5</v>
-      </c>
-      <c r="I2" s="4">
+      <c r="H2" s="8">
+        <v>5</v>
+      </c>
+      <c r="I2" s="8">
         <v>6</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="8">
         <v>7</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2" s="8">
         <v>8</v>
       </c>
-      <c r="L2" s="4">
+      <c r="L2" s="21">
         <v>9</v>
       </c>
-      <c r="N2" t="s">
-        <v>16</v>
-      </c>
+      <c r="M2" s="35"/>
+      <c r="N2" s="37"/>
       <c r="Q2" t="s">
         <v>18</v>
       </c>
-      <c r="R2" s="5">
-        <v>3.8899999999999997E-2</v>
+      <c r="R2" s="4">
+        <f>N13/M13</f>
+        <v>3.9399999999999998E-2</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="18">
         <v>0</v>
       </c>
-      <c r="C3">
-        <v>967</v>
-      </c>
-      <c r="D3">
+      <c r="C3" s="12">
+        <v>969</v>
+      </c>
+      <c r="D3" s="13">
         <v>0</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="13">
+        <v>2</v>
+      </c>
+      <c r="F3" s="13">
+        <v>0</v>
+      </c>
+      <c r="G3" s="13">
+        <v>0</v>
+      </c>
+      <c r="H3" s="13">
+        <v>2</v>
+      </c>
+      <c r="I3" s="13">
+        <v>4</v>
+      </c>
+      <c r="J3" s="13">
+        <v>1</v>
+      </c>
+      <c r="K3" s="13">
+        <v>2</v>
+      </c>
+      <c r="L3" s="22">
+        <v>0</v>
+      </c>
+      <c r="M3" s="26">
+        <f>SUM(C3:L3)</f>
+        <v>980</v>
+      </c>
+      <c r="N3" s="14">
+        <f>M3-C3</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="29"/>
+      <c r="B4" s="19">
+        <v>1</v>
+      </c>
+      <c r="C4" s="16">
+        <v>0</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1121</v>
+      </c>
+      <c r="E4" s="6">
+        <v>3</v>
+      </c>
+      <c r="F4" s="6">
+        <v>2</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0</v>
+      </c>
+      <c r="H4" s="6">
+        <v>1</v>
+      </c>
+      <c r="I4" s="6">
+        <v>5</v>
+      </c>
+      <c r="J4" s="6">
+        <v>1</v>
+      </c>
+      <c r="K4" s="6">
+        <v>2</v>
+      </c>
+      <c r="L4" s="23">
+        <v>0</v>
+      </c>
+      <c r="M4" s="5">
+        <f t="shared" ref="M4:M12" si="0">SUM(C4:L4)</f>
+        <v>1135</v>
+      </c>
+      <c r="N4" s="7">
+        <f>M4-D4</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="29"/>
+      <c r="B5" s="19">
+        <v>2</v>
+      </c>
+      <c r="C5" s="16">
         <v>9</v>
       </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="G3">
+      <c r="D5" s="6">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6">
+        <v>985</v>
+      </c>
+      <c r="F5" s="6">
+        <v>7</v>
+      </c>
+      <c r="G5" s="6">
         <v>1</v>
       </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="I3">
+      <c r="H5" s="6">
+        <v>0</v>
+      </c>
+      <c r="I5" s="6">
+        <v>1</v>
+      </c>
+      <c r="J5" s="6">
         <v>9</v>
       </c>
-      <c r="J3">
+      <c r="K5" s="6">
+        <v>20</v>
+      </c>
+      <c r="L5" s="23">
         <v>0</v>
       </c>
-      <c r="K3">
-        <v>3</v>
-      </c>
-      <c r="L3">
-        <v>8</v>
-      </c>
-      <c r="M3">
-        <f>SUM(C3:L3)</f>
-        <v>1001</v>
-      </c>
-      <c r="N3">
-        <f>M3-C3</f>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>1122</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>3</v>
-      </c>
-      <c r="J4">
-        <v>5</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>6</v>
-      </c>
-      <c r="M4">
-        <f t="shared" ref="M4:M12" si="0">SUM(C4:L4)</f>
-        <v>1137</v>
-      </c>
-      <c r="N4">
-        <f>M4-D4</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="4">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5">
-        <v>987</v>
-      </c>
-      <c r="F5">
-        <v>7</v>
-      </c>
-      <c r="G5">
-        <v>5</v>
-      </c>
-      <c r="H5">
-        <v>3</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>17</v>
-      </c>
-      <c r="K5">
-        <v>7</v>
-      </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="M5">
+      <c r="M5" s="5">
         <f t="shared" si="0"/>
         <v>1032</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="7">
         <f>M5-E5</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="29"/>
+      <c r="B6" s="19">
+        <v>3</v>
+      </c>
+      <c r="C6" s="16">
+        <v>2</v>
+      </c>
+      <c r="D6" s="6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="6">
+        <v>5</v>
+      </c>
+      <c r="F6" s="6">
+        <v>966</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="6">
+        <v>8</v>
+      </c>
+      <c r="I6" s="6">
+        <v>2</v>
+      </c>
+      <c r="J6" s="6">
+        <v>12</v>
+      </c>
+      <c r="K6" s="6">
+        <v>11</v>
+      </c>
+      <c r="L6" s="23">
+        <v>3</v>
+      </c>
+      <c r="M6" s="5">
+        <f t="shared" si="0"/>
+        <v>1010</v>
+      </c>
+      <c r="N6" s="7">
+        <f>M6-F6</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="29"/>
+      <c r="B7" s="19">
+        <v>4</v>
+      </c>
+      <c r="C7" s="16">
+        <v>1</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0</v>
+      </c>
+      <c r="E7" s="6">
+        <v>6</v>
+      </c>
+      <c r="F7" s="6">
+        <v>0</v>
+      </c>
+      <c r="G7" s="6">
+        <v>946</v>
+      </c>
+      <c r="H7" s="6">
+        <v>1</v>
+      </c>
+      <c r="I7" s="6">
+        <v>7</v>
+      </c>
+      <c r="J7" s="6">
+        <v>1</v>
+      </c>
+      <c r="K7" s="6">
+        <v>3</v>
+      </c>
+      <c r="L7" s="23">
+        <v>17</v>
+      </c>
+      <c r="M7" s="5">
+        <f t="shared" si="0"/>
+        <v>982</v>
+      </c>
+      <c r="N7" s="7">
+        <f>M7-G7</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="29"/>
+      <c r="B8" s="19">
+        <v>5</v>
+      </c>
+      <c r="C8" s="16">
+        <v>3</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0</v>
+      </c>
+      <c r="E8" s="6">
+        <v>4</v>
+      </c>
+      <c r="F8" s="6">
+        <v>18</v>
+      </c>
+      <c r="G8" s="6">
+        <v>7</v>
+      </c>
+      <c r="H8" s="6">
+        <v>847</v>
+      </c>
+      <c r="I8" s="6">
+        <v>7</v>
+      </c>
+      <c r="J8" s="6">
+        <v>1</v>
+      </c>
+      <c r="K8" s="6">
+        <v>3</v>
+      </c>
+      <c r="L8" s="23">
+        <v>2</v>
+      </c>
+      <c r="M8" s="5">
+        <f t="shared" si="0"/>
+        <v>892</v>
+      </c>
+      <c r="N8" s="7">
+        <f>M8-H8</f>
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="4">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="29"/>
+      <c r="B9" s="19">
+        <v>6</v>
+      </c>
+      <c r="C9" s="16">
+        <v>9</v>
+      </c>
+      <c r="D9" s="6">
         <v>3</v>
       </c>
-      <c r="C6">
+      <c r="E9" s="6">
         <v>0</v>
       </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6">
-        <v>5</v>
-      </c>
-      <c r="F6">
-        <v>966</v>
-      </c>
-      <c r="G6">
+      <c r="F9" s="6">
         <v>0</v>
       </c>
-      <c r="H6">
-        <v>16</v>
-      </c>
-      <c r="I6">
+      <c r="G9" s="6">
+        <v>2</v>
+      </c>
+      <c r="H9" s="6">
+        <v>3</v>
+      </c>
+      <c r="I9" s="6">
+        <v>940</v>
+      </c>
+      <c r="J9" s="6">
         <v>0</v>
       </c>
-      <c r="J6">
+      <c r="K9" s="6">
+        <v>1</v>
+      </c>
+      <c r="L9" s="23">
         <v>0</v>
       </c>
-      <c r="K6">
+      <c r="M9" s="5">
+        <f t="shared" si="0"/>
+        <v>958</v>
+      </c>
+      <c r="N9" s="7">
+        <f>M9-I9</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="29"/>
+      <c r="B10" s="19">
+        <v>7</v>
+      </c>
+      <c r="C10" s="16">
+        <v>0</v>
+      </c>
+      <c r="D10" s="6">
+        <v>5</v>
+      </c>
+      <c r="E10" s="6">
         <v>17</v>
       </c>
-      <c r="L6">
-        <v>14</v>
-      </c>
-      <c r="M6">
+      <c r="F10" s="6">
+        <v>0</v>
+      </c>
+      <c r="G10" s="6">
+        <v>5</v>
+      </c>
+      <c r="H10" s="6">
+        <v>0</v>
+      </c>
+      <c r="I10" s="6">
+        <v>0</v>
+      </c>
+      <c r="J10" s="6">
+        <v>979</v>
+      </c>
+      <c r="K10" s="6">
+        <v>4</v>
+      </c>
+      <c r="L10" s="23">
+        <v>18</v>
+      </c>
+      <c r="M10" s="5">
         <f t="shared" si="0"/>
-        <v>1020</v>
-      </c>
-      <c r="N6">
-        <f>M6-F6</f>
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="4">
+        <v>1028</v>
+      </c>
+      <c r="N10" s="7">
+        <f>M10-J10</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="29"/>
+      <c r="B11" s="19">
+        <v>8</v>
+      </c>
+      <c r="C11" s="16">
         <v>4</v>
       </c>
-      <c r="C7">
+      <c r="D11" s="6">
         <v>0</v>
       </c>
-      <c r="D7">
+      <c r="E11" s="6">
+        <v>5</v>
+      </c>
+      <c r="F11" s="6">
+        <v>17</v>
+      </c>
+      <c r="G11" s="6">
+        <v>11</v>
+      </c>
+      <c r="H11" s="6">
+        <v>10</v>
+      </c>
+      <c r="I11" s="6">
+        <v>4</v>
+      </c>
+      <c r="J11" s="6">
+        <v>7</v>
+      </c>
+      <c r="K11" s="6">
+        <v>911</v>
+      </c>
+      <c r="L11" s="23">
+        <v>5</v>
+      </c>
+      <c r="M11" s="5">
+        <f t="shared" si="0"/>
+        <v>974</v>
+      </c>
+      <c r="N11" s="7">
+        <f>M11-K11</f>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="30"/>
+      <c r="B12" s="20">
+        <v>9</v>
+      </c>
+      <c r="C12" s="17">
+        <v>8</v>
+      </c>
+      <c r="D12" s="9">
+        <v>7</v>
+      </c>
+      <c r="E12" s="9">
+        <v>2</v>
+      </c>
+      <c r="F12" s="9">
+        <v>13</v>
+      </c>
+      <c r="G12" s="9">
+        <v>19</v>
+      </c>
+      <c r="H12" s="9">
+        <v>3</v>
+      </c>
+      <c r="I12" s="9">
         <v>0</v>
       </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>948</v>
-      </c>
-      <c r="H7">
-        <v>7</v>
-      </c>
-      <c r="I7">
-        <v>3</v>
-      </c>
-      <c r="J7">
-        <v>5</v>
-      </c>
-      <c r="K7">
-        <v>10</v>
-      </c>
-      <c r="L7">
-        <v>19</v>
-      </c>
-      <c r="M7">
+      <c r="J12" s="9">
+        <v>11</v>
+      </c>
+      <c r="K12" s="9">
+        <v>4</v>
+      </c>
+      <c r="L12" s="24">
+        <v>942</v>
+      </c>
+      <c r="M12" s="25">
         <f t="shared" si="0"/>
-        <v>993</v>
-      </c>
-      <c r="N7">
-        <f>M7-G7</f>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="4">
-        <v>5</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>6</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>848</v>
-      </c>
-      <c r="I8">
-        <v>4</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>10</v>
-      </c>
-      <c r="L8">
-        <v>4</v>
-      </c>
-      <c r="M8">
-        <f t="shared" si="0"/>
-        <v>875</v>
-      </c>
-      <c r="N8">
-        <f>M8-H8</f>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="4">
-        <v>6</v>
-      </c>
-      <c r="C9">
-        <v>5</v>
-      </c>
-      <c r="D9">
-        <v>4</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>2</v>
-      </c>
-      <c r="G9">
-        <v>8</v>
-      </c>
-      <c r="H9">
-        <v>9</v>
-      </c>
-      <c r="I9">
-        <v>938</v>
-      </c>
-      <c r="J9">
-        <v>1</v>
-      </c>
-      <c r="K9">
-        <v>3</v>
-      </c>
-      <c r="L9">
-        <v>1</v>
-      </c>
-      <c r="M9">
-        <f t="shared" si="0"/>
-        <v>972</v>
-      </c>
-      <c r="N9">
-        <f>M9-I9</f>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="4">
-        <v>7</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>9</v>
-      </c>
-      <c r="F10">
-        <v>12</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>2</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>978</v>
-      </c>
-      <c r="K10">
-        <v>6</v>
-      </c>
-      <c r="L10">
-        <v>9</v>
-      </c>
-      <c r="M10">
-        <f t="shared" si="0"/>
-        <v>1019</v>
-      </c>
-      <c r="N10">
-        <f>M10-J10</f>
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="4">
-        <v>8</v>
-      </c>
-      <c r="C11">
-        <v>3</v>
-      </c>
-      <c r="D11">
-        <v>2</v>
-      </c>
-      <c r="E11">
-        <v>20</v>
-      </c>
-      <c r="F11">
-        <v>11</v>
-      </c>
-      <c r="G11">
-        <v>4</v>
-      </c>
-      <c r="H11">
-        <v>3</v>
-      </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-      <c r="J11">
-        <v>3</v>
-      </c>
-      <c r="K11">
-        <v>912</v>
-      </c>
-      <c r="L11">
-        <v>2</v>
-      </c>
-      <c r="M11">
-        <f t="shared" si="0"/>
-        <v>961</v>
-      </c>
-      <c r="N11">
-        <f>M11-K11</f>
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="4">
-        <v>9</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>3</v>
-      </c>
-      <c r="G12">
-        <v>15</v>
-      </c>
-      <c r="H12">
-        <v>2</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>19</v>
-      </c>
-      <c r="K12">
-        <v>6</v>
-      </c>
-      <c r="L12">
-        <v>945</v>
-      </c>
-      <c r="M12">
-        <f t="shared" si="0"/>
-        <v>990</v>
-      </c>
-      <c r="N12">
+        <v>1009</v>
+      </c>
+      <c r="N12" s="10">
         <f>M12-L12</f>
-        <v>45</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -17675,14 +18216,20 @@
         <v>13</v>
       </c>
       <c r="M13">
-        <f t="shared" ref="M13" si="1">SUM(M3:M12)</f>
+        <f t="shared" ref="M13:N13" si="1">SUM(M3:M12)</f>
         <v>10000</v>
       </c>
+      <c r="N13">
+        <f t="shared" si="1"/>
+        <v>394</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A3:A12"/>
     <mergeCell ref="C1:L1"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:N2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -17695,509 +18242,524 @@
   <dimension ref="A1:R13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="12" width="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7" customWidth="1"/>
+    <col min="14" max="14" width="8" customWidth="1"/>
     <col min="17" max="17" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C1" s="8" t="s">
+      <c r="A1" s="11"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C2" s="4">
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="36"/>
+    </row>
+    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="15">
         <v>0</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="8">
         <v>1</v>
       </c>
-      <c r="E2" s="4">
-        <v>2</v>
-      </c>
-      <c r="F2" s="4">
+      <c r="E2" s="8">
+        <v>2</v>
+      </c>
+      <c r="F2" s="8">
         <v>3</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="8">
         <v>4</v>
       </c>
-      <c r="H2" s="4">
-        <v>5</v>
-      </c>
-      <c r="I2" s="4">
+      <c r="H2" s="8">
+        <v>5</v>
+      </c>
+      <c r="I2" s="8">
         <v>6</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="8">
         <v>7</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2" s="8">
         <v>8</v>
       </c>
-      <c r="L2" s="4">
+      <c r="L2" s="21">
         <v>9</v>
       </c>
-      <c r="N2" t="s">
+      <c r="M2" s="35"/>
+      <c r="N2" s="37" t="s">
         <v>16</v>
       </c>
       <c r="Q2" t="s">
         <v>17</v>
       </c>
-      <c r="R2" s="5">
-        <v>4.1099999999999998E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="R2" s="4">
+        <f>N13/M13</f>
+        <v>4.1500000000000002E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="18">
         <v>0</v>
       </c>
-      <c r="C3">
-        <v>968</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
+      <c r="C3" s="12">
+        <v>969</v>
+      </c>
+      <c r="D3" s="13">
+        <v>0</v>
+      </c>
+      <c r="E3" s="13">
+        <v>1</v>
+      </c>
+      <c r="F3" s="13">
+        <v>0</v>
+      </c>
+      <c r="G3" s="13">
+        <v>2</v>
+      </c>
+      <c r="H3" s="13">
+        <v>1</v>
+      </c>
+      <c r="I3" s="13">
+        <v>4</v>
+      </c>
+      <c r="J3" s="13">
+        <v>2</v>
+      </c>
+      <c r="K3" s="13">
+        <v>1</v>
+      </c>
+      <c r="L3" s="22">
+        <v>0</v>
+      </c>
+      <c r="M3" s="26">
+        <f>SUM(C3:L3)</f>
+        <v>980</v>
+      </c>
+      <c r="N3" s="14">
+        <f>M3-C3</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="29"/>
+      <c r="B4" s="19">
+        <v>1</v>
+      </c>
+      <c r="C4" s="16">
+        <v>2</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1118</v>
+      </c>
+      <c r="E4" s="6">
         <v>6</v>
       </c>
-      <c r="F3">
+      <c r="F4" s="6">
+        <v>2</v>
+      </c>
+      <c r="G4" s="6">
         <v>0</v>
       </c>
-      <c r="G3">
+      <c r="H4" s="6">
+        <v>1</v>
+      </c>
+      <c r="I4" s="6">
+        <v>2</v>
+      </c>
+      <c r="J4" s="6">
         <v>0</v>
       </c>
-      <c r="H3">
-        <v>4</v>
-      </c>
-      <c r="I3">
-        <v>12</v>
-      </c>
-      <c r="J3">
-        <v>2</v>
-      </c>
-      <c r="K3">
-        <v>11</v>
-      </c>
-      <c r="L3">
-        <v>9</v>
-      </c>
-      <c r="M3">
-        <f>SUM(C3:L3)</f>
-        <v>1014</v>
-      </c>
-      <c r="N3">
-        <f>M3-C3</f>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="4">
+      <c r="K4" s="6">
+        <v>3</v>
+      </c>
+      <c r="L4" s="23">
         <v>1</v>
       </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>1119</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>4</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>2</v>
-      </c>
-      <c r="J4">
-        <v>5</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>5</v>
-      </c>
-      <c r="M4">
+      <c r="M4" s="5">
         <f t="shared" ref="M4:M12" si="0">SUM(C4:L4)</f>
         <v>1135</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="7">
         <f>M4-D4</f>
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="4">
-        <v>2</v>
-      </c>
-      <c r="C5">
+      <c r="A5" s="29"/>
+      <c r="B5" s="19">
+        <v>2</v>
+      </c>
+      <c r="C5" s="16">
+        <v>8</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6">
+        <v>991</v>
+      </c>
+      <c r="F5" s="6">
+        <v>10</v>
+      </c>
+      <c r="G5" s="6">
         <v>1</v>
       </c>
-      <c r="D5">
+      <c r="H5" s="6">
+        <v>0</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0</v>
+      </c>
+      <c r="J5" s="6">
+        <v>9</v>
+      </c>
+      <c r="K5" s="6">
+        <v>12</v>
+      </c>
+      <c r="L5" s="23">
+        <v>1</v>
+      </c>
+      <c r="M5" s="5">
+        <f t="shared" si="0"/>
+        <v>1032</v>
+      </c>
+      <c r="N5" s="7">
+        <f>M5-E5</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="29"/>
+      <c r="B6" s="19">
+        <v>3</v>
+      </c>
+      <c r="C6" s="16">
+        <v>0</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="6">
         <v>7</v>
       </c>
-      <c r="E5">
-        <v>992</v>
-      </c>
-      <c r="F5">
-        <v>11</v>
-      </c>
-      <c r="G5">
+      <c r="F6" s="6">
+        <v>985</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="6">
+        <v>1</v>
+      </c>
+      <c r="I6" s="6">
+        <v>0</v>
+      </c>
+      <c r="J6" s="6">
+        <v>6</v>
+      </c>
+      <c r="K6" s="6">
+        <v>6</v>
+      </c>
+      <c r="L6" s="23">
+        <v>5</v>
+      </c>
+      <c r="M6" s="5">
+        <f t="shared" si="0"/>
+        <v>1010</v>
+      </c>
+      <c r="N6" s="7">
+        <f>M6-F6</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="29"/>
+      <c r="B7" s="19">
+        <v>4</v>
+      </c>
+      <c r="C7" s="16">
+        <v>0</v>
+      </c>
+      <c r="D7" s="6">
+        <v>4</v>
+      </c>
+      <c r="E7" s="6">
         <v>3</v>
       </c>
-      <c r="H5">
+      <c r="F7" s="6">
+        <v>0</v>
+      </c>
+      <c r="G7" s="6">
+        <v>931</v>
+      </c>
+      <c r="H7" s="6">
+        <v>0</v>
+      </c>
+      <c r="I7" s="6">
+        <v>8</v>
+      </c>
+      <c r="J7" s="6">
+        <v>2</v>
+      </c>
+      <c r="K7" s="6">
+        <v>3</v>
+      </c>
+      <c r="L7" s="23">
+        <v>31</v>
+      </c>
+      <c r="M7" s="5">
+        <f t="shared" si="0"/>
+        <v>982</v>
+      </c>
+      <c r="N7" s="7">
+        <f>M7-G7</f>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="29"/>
+      <c r="B8" s="19">
+        <v>5</v>
+      </c>
+      <c r="C8" s="16">
+        <v>6</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0</v>
+      </c>
+      <c r="E8" s="6">
+        <v>5</v>
+      </c>
+      <c r="F8" s="6">
+        <v>23</v>
+      </c>
+      <c r="G8" s="6">
+        <v>2</v>
+      </c>
+      <c r="H8" s="6">
+        <v>833</v>
+      </c>
+      <c r="I8" s="6">
+        <v>12</v>
+      </c>
+      <c r="J8" s="6">
+        <v>2</v>
+      </c>
+      <c r="K8" s="6">
+        <v>6</v>
+      </c>
+      <c r="L8" s="23">
+        <v>3</v>
+      </c>
+      <c r="M8" s="5">
+        <f t="shared" si="0"/>
+        <v>892</v>
+      </c>
+      <c r="N8" s="7">
+        <f>M8-H8</f>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="29"/>
+      <c r="B9" s="19">
+        <v>6</v>
+      </c>
+      <c r="C9" s="16">
+        <v>15</v>
+      </c>
+      <c r="D9" s="6">
+        <v>2</v>
+      </c>
+      <c r="E9" s="6">
+        <v>0</v>
+      </c>
+      <c r="F9" s="6">
+        <v>0</v>
+      </c>
+      <c r="G9" s="6">
+        <v>5</v>
+      </c>
+      <c r="H9" s="6">
+        <v>9</v>
+      </c>
+      <c r="I9" s="6">
+        <v>926</v>
+      </c>
+      <c r="J9" s="6">
+        <v>0</v>
+      </c>
+      <c r="K9" s="6">
+        <v>1</v>
+      </c>
+      <c r="L9" s="23">
+        <v>0</v>
+      </c>
+      <c r="M9" s="5">
+        <f t="shared" si="0"/>
+        <v>958</v>
+      </c>
+      <c r="N9" s="7">
+        <f>M9-I9</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="29"/>
+      <c r="B10" s="19">
+        <v>7</v>
+      </c>
+      <c r="C10" s="16">
+        <v>2</v>
+      </c>
+      <c r="D10" s="6">
+        <v>5</v>
+      </c>
+      <c r="E10" s="6">
+        <v>24</v>
+      </c>
+      <c r="F10" s="6">
+        <v>1</v>
+      </c>
+      <c r="G10" s="6">
+        <v>13</v>
+      </c>
+      <c r="H10" s="6">
+        <v>0</v>
+      </c>
+      <c r="I10" s="6">
+        <v>0</v>
+      </c>
+      <c r="J10" s="6">
+        <v>958</v>
+      </c>
+      <c r="K10" s="6">
         <v>4</v>
       </c>
-      <c r="I5">
+      <c r="L10" s="23">
+        <v>21</v>
+      </c>
+      <c r="M10" s="5">
+        <f t="shared" si="0"/>
+        <v>1028</v>
+      </c>
+      <c r="N10" s="7">
+        <f>M10-J10</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="29"/>
+      <c r="B11" s="19">
+        <v>8</v>
+      </c>
+      <c r="C11" s="16">
+        <v>12</v>
+      </c>
+      <c r="D11" s="6">
         <v>1</v>
       </c>
-      <c r="J5">
-        <v>24</v>
-      </c>
-      <c r="K5">
+      <c r="E11" s="6">
         <v>7</v>
       </c>
-      <c r="L5">
+      <c r="F11" s="6">
+        <v>12</v>
+      </c>
+      <c r="G11" s="6">
+        <v>6</v>
+      </c>
+      <c r="H11" s="6">
+        <v>7</v>
+      </c>
+      <c r="I11" s="6">
         <v>3</v>
       </c>
-      <c r="M5">
+      <c r="J11" s="6">
+        <v>6</v>
+      </c>
+      <c r="K11" s="6">
+        <v>918</v>
+      </c>
+      <c r="L11" s="23">
+        <v>2</v>
+      </c>
+      <c r="M11" s="5">
         <f t="shared" si="0"/>
-        <v>1053</v>
-      </c>
-      <c r="N5">
-        <f>M5-E5</f>
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="4">
+        <v>974</v>
+      </c>
+      <c r="N11" s="7">
+        <f>M11-K11</f>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="30"/>
+      <c r="B12" s="20">
+        <v>9</v>
+      </c>
+      <c r="C12" s="17">
+        <v>9</v>
+      </c>
+      <c r="D12" s="9">
+        <v>5</v>
+      </c>
+      <c r="E12" s="9">
+        <v>2</v>
+      </c>
+      <c r="F12" s="9">
+        <v>14</v>
+      </c>
+      <c r="G12" s="9">
+        <v>7</v>
+      </c>
+      <c r="H12" s="9">
+        <v>1</v>
+      </c>
+      <c r="I12" s="9">
+        <v>0</v>
+      </c>
+      <c r="J12" s="9">
+        <v>12</v>
+      </c>
+      <c r="K12" s="9">
         <v>3</v>
       </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>8</v>
-      </c>
-      <c r="F6">
-        <v>981</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>22</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>2</v>
-      </c>
-      <c r="K6">
-        <v>9</v>
-      </c>
-      <c r="L6">
-        <v>15</v>
-      </c>
-      <c r="M6">
+      <c r="L12" s="24">
+        <v>956</v>
+      </c>
+      <c r="M12" s="25">
         <f t="shared" si="0"/>
-        <v>1038</v>
-      </c>
-      <c r="N6">
-        <f>M6-F6</f>
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="4">
-        <v>4</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>930</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7">
-        <v>3</v>
-      </c>
-      <c r="J7">
-        <v>11</v>
-      </c>
-      <c r="K7">
-        <v>7</v>
-      </c>
-      <c r="L7">
-        <v>8</v>
-      </c>
-      <c r="M7">
-        <f t="shared" si="0"/>
-        <v>962</v>
-      </c>
-      <c r="N7">
-        <f>M7-G7</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="4">
-        <v>5</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>839</v>
-      </c>
-      <c r="I8">
-        <v>8</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>4</v>
-      </c>
-      <c r="L8">
-        <v>3</v>
-      </c>
-      <c r="M8">
-        <f t="shared" si="0"/>
-        <v>858</v>
-      </c>
-      <c r="N8">
-        <f>M8-H8</f>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="4">
-        <v>6</v>
-      </c>
-      <c r="C9">
-        <v>5</v>
-      </c>
-      <c r="D9">
-        <v>3</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>6</v>
-      </c>
-      <c r="H9">
-        <v>9</v>
-      </c>
-      <c r="I9">
-        <v>929</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>2</v>
-      </c>
-      <c r="L9">
-        <v>1</v>
-      </c>
-      <c r="M9">
-        <f t="shared" si="0"/>
-        <v>955</v>
-      </c>
-      <c r="N9">
-        <f>M9-I9</f>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="4">
-        <v>7</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>11</v>
-      </c>
-      <c r="F10">
-        <v>8</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>3</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>959</v>
-      </c>
-      <c r="K10">
-        <v>8</v>
-      </c>
-      <c r="L10">
-        <v>13</v>
-      </c>
-      <c r="M10">
-        <f t="shared" si="0"/>
-        <v>1004</v>
-      </c>
-      <c r="N10">
-        <f>M10-J10</f>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="4">
-        <v>8</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>2</v>
-      </c>
-      <c r="E11">
-        <v>15</v>
-      </c>
-      <c r="F11">
-        <v>5</v>
-      </c>
-      <c r="G11">
-        <v>2</v>
-      </c>
-      <c r="H11">
-        <v>6</v>
-      </c>
-      <c r="I11">
-        <v>2</v>
-      </c>
-      <c r="J11">
-        <v>5</v>
-      </c>
-      <c r="K11">
-        <v>923</v>
-      </c>
-      <c r="L11">
-        <v>3</v>
-      </c>
-      <c r="M11">
-        <f t="shared" si="0"/>
-        <v>964</v>
-      </c>
-      <c r="N11">
-        <f>M11-K11</f>
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="4">
-        <v>9</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>4</v>
-      </c>
-      <c r="G12">
-        <v>36</v>
-      </c>
-      <c r="H12">
-        <v>4</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-      <c r="J12">
-        <v>20</v>
-      </c>
-      <c r="K12">
-        <v>3</v>
-      </c>
-      <c r="L12">
-        <v>949</v>
-      </c>
-      <c r="M12">
-        <f t="shared" si="0"/>
-        <v>1017</v>
-      </c>
-      <c r="N12">
+        <v>1009</v>
+      </c>
+      <c r="N12" s="10">
         <f>M12-L12</f>
-        <v>68</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -18205,14 +18767,20 @@
         <v>13</v>
       </c>
       <c r="M13">
-        <f t="shared" ref="M13" si="1">SUM(M3:M12)</f>
+        <f t="shared" ref="M13:N13" si="1">SUM(M3:M12)</f>
         <v>10000</v>
       </c>
+      <c r="N13">
+        <f t="shared" si="1"/>
+        <v>415</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="C1:L1"/>
     <mergeCell ref="A3:A12"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:N2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>